<commit_message>
fix(test case 1): refactored test data
</commit_message>
<xml_diff>
--- a/Test Case 1.xlsx
+++ b/Test Case 1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shahriar/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1222290D-37DD-3F45-8050-37B26E971593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21510" windowHeight="12225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21520" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="67">
   <si>
     <t>TC No</t>
   </si>
@@ -75,9 +76,6 @@
   </si>
   <si>
     <t>Check the field take only number or not</t>
-  </si>
-  <si>
-    <t>123456789,mounota321</t>
   </si>
   <si>
     <t>Cannot Register</t>
@@ -233,7 +231,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -280,7 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -307,14 +305,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -597,66 +592,66 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" customWidth="1"/>
-    <col min="6" max="6" width="55.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="6.5" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="30.5" customWidth="1"/>
+    <col min="6" max="6" width="55.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="11" t="s">
+      <c r="D1" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>12</v>
       </c>
       <c r="E2" t="s">
@@ -672,20 +667,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
       <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5">
+        <v>123456789</v>
+      </c>
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
@@ -694,20 +689,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -716,20 +711,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
+    <row r="5" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
@@ -738,20 +733,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
         <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -760,54 +755,54 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="12">
         <v>2</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>28</v>
+      <c r="B7" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="5">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" t="s">
         <v>32</v>
       </c>
-      <c r="G7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
       <c r="C9" t="s">
         <v>11</v>
       </c>
@@ -815,229 +810,229 @@
         <v>12</v>
       </c>
       <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
         <v>36</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="9" t="s">
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" t="s">
         <v>40</v>
       </c>
-      <c r="G10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D11" t="s">
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="12">
+        <v>3</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>3</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G13" t="s">
         <v>9</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" t="s">
         <v>52</v>
       </c>
-      <c r="F14" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="D15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="F15" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="12">
+        <v>4</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
         <v>55</v>
       </c>
-      <c r="G15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>4</v>
-      </c>
-      <c r="B16" s="10" t="s">
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" t="s">
-        <v>51</v>
-      </c>
-      <c r="H16" s="1" t="s">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" t="s">
-        <v>61</v>
       </c>
       <c r="D17" s="6">
         <v>36594157823</v>
       </c>
       <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="F17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G17" t="s">
-        <v>51</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" t="s">
-        <v>51</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="G19" t="s">
         <v>9</v>
@@ -1055,40 +1050,40 @@
     <mergeCell ref="A16:A19"/>
   </mergeCells>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G12" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$G$2:$G$12</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G13:G14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G13:G14" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$G$13:$G$30</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G15" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>$G$15:$G$30</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G16" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>G16:G22</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G17" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>$G$17:$G$22</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G19" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>$G$15:$G$22</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H4" r:id="rId3"/>
-    <hyperlink ref="H5" r:id="rId4"/>
-    <hyperlink ref="H6" r:id="rId5"/>
-    <hyperlink ref="H7" r:id="rId6"/>
-    <hyperlink ref="H10" r:id="rId7"/>
-    <hyperlink ref="H11" r:id="rId8"/>
-    <hyperlink ref="H13" r:id="rId9"/>
-    <hyperlink ref="H15" r:id="rId10"/>
-    <hyperlink ref="D15" r:id="rId11"/>
-    <hyperlink ref="H16" r:id="rId12" display="Mobil"/>
-    <hyperlink ref="H17" r:id="rId13"/>
-    <hyperlink ref="H18" r:id="rId14"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="H15" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="H16" r:id="rId12" display="Mobil" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="H17" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="H18" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>

</xml_diff>